<commit_message>
Continue, with new empty template
</commit_message>
<xml_diff>
--- a/doc/template_files/krstenica-template.xlsx
+++ b/doc/template_files/krstenica-template.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">          у</t>
+    <t xml:space="preserve">   у</t>
   </si>
   <si>
     <t xml:space="preserve">        за </t>
@@ -134,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -194,6 +194,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,7 +210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -219,6 +225,15 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -248,7 +263,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,7 +288,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,10 +322,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:M66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.48828125" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -310,6 +337,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="13.47"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="76.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -324,7 +352,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -336,7 +364,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -367,7 +395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -382,7 +410,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -392,20 +420,20 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="4"/>
+      <c r="M11" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -419,14 +447,15 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -440,12 +469,13 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -459,12 +489,13 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
@@ -755,11 +786,10 @@
       <c r="L66" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="E2:J4"/>
     <mergeCell ref="C9:L9"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="H11:I11"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="I64:K64"/>

</xml_diff>